<commit_message>
feat: the first card using OJ worked!
</commit_message>
<xml_diff>
--- a/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
+++ b/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\iyingdiBattleGround\iyingdiBattleGround\Assets\StreamingAssets\Mods\Buildin\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5165B-5DF7-4D76-94F8-C34E99771F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1156A42-582F-47A7-B8C9-5760A1AFD45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="591">
   <si>
     <t>鱼人招潮者</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1749,10 +1749,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WhenMinionSummon: if:target.isType:"鱼人": host.AddBuff:“加一攻”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//唯一名称0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1818,6 +1814,14 @@
   </si>
   <si>
     <t>Buff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log: "鱼人领军init"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"if:1,1"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2146,13 +2150,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2171,52 +2176,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B1" t="s">
         <v>573</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>574</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>575</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>576</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>577</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>578</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>579</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>582</v>
+      </c>
+      <c r="J1" t="s">
+        <v>583</v>
+      </c>
+      <c r="K1" t="s">
+        <v>584</v>
+      </c>
+      <c r="L1" t="s">
+        <v>585</v>
+      </c>
+      <c r="M1" t="s">
+        <v>586</v>
+      </c>
+      <c r="N1" t="s">
+        <v>587</v>
+      </c>
+      <c r="O1" t="s">
         <v>580</v>
       </c>
-      <c r="I1" t="s">
-        <v>583</v>
-      </c>
-      <c r="J1" t="s">
-        <v>584</v>
-      </c>
-      <c r="K1" t="s">
-        <v>585</v>
-      </c>
-      <c r="L1" t="s">
-        <v>586</v>
-      </c>
-      <c r="M1" t="s">
-        <v>587</v>
-      </c>
-      <c r="N1" t="s">
-        <v>588</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>581</v>
-      </c>
-      <c r="P1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>6</v>
@@ -2282,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2315,6 +2320,9 @@
       </c>
       <c r="K5" s="1">
         <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>589</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Revert "feat: the first card using OJ worked!"
This reverts commit 4034081372bc58a6ce59a046b68365ac960b540c.
</commit_message>
<xml_diff>
--- a/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
+++ b/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\iyingdiBattleGround\iyingdiBattleGround\Assets\StreamingAssets\Mods\Buildin\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1156A42-582F-47A7-B8C9-5760A1AFD45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5165B-5DF7-4D76-94F8-C34E99771F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="590">
   <si>
     <t>鱼人招潮者</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1749,6 +1749,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>WhenMinionSummon: if:target.isType:"鱼人": host.AddBuff:“加一攻”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>//唯一名称0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1814,14 +1818,6 @@
   </si>
   <si>
     <t>Buff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Log: "鱼人领军init"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"if:1,1"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2150,14 +2146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2176,52 +2171,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="I1" t="s">
+        <v>583</v>
+      </c>
+      <c r="J1" t="s">
+        <v>584</v>
+      </c>
+      <c r="K1" t="s">
+        <v>585</v>
+      </c>
+      <c r="L1" t="s">
+        <v>586</v>
+      </c>
+      <c r="M1" t="s">
+        <v>587</v>
+      </c>
+      <c r="N1" t="s">
+        <v>588</v>
+      </c>
+      <c r="O1" t="s">
+        <v>581</v>
+      </c>
+      <c r="P1" t="s">
         <v>582</v>
-      </c>
-      <c r="J1" t="s">
-        <v>583</v>
-      </c>
-      <c r="K1" t="s">
-        <v>584</v>
-      </c>
-      <c r="L1" t="s">
-        <v>585</v>
-      </c>
-      <c r="M1" t="s">
-        <v>586</v>
-      </c>
-      <c r="N1" t="s">
-        <v>587</v>
-      </c>
-      <c r="O1" t="s">
-        <v>580</v>
-      </c>
-      <c r="P1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2271,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>6</v>
@@ -2287,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2320,9 +2315,6 @@
       </c>
       <c r="K5" s="1">
         <v>3</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>589</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Revert "Revert "feat: the first card using OJ worked!""
This reverts commit e2c5a688b625e61945e34bc75b57a259fd785e49.
</commit_message>
<xml_diff>
--- a/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
+++ b/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\iyingdiBattleGround\iyingdiBattleGround\Assets\StreamingAssets\Mods\Buildin\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5165B-5DF7-4D76-94F8-C34E99771F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1156A42-582F-47A7-B8C9-5760A1AFD45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="591">
   <si>
     <t>鱼人招潮者</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1749,10 +1749,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WhenMinionSummon: if:target.isType:"鱼人": host.AddBuff:“加一攻”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//唯一名称0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1818,6 +1814,14 @@
   </si>
   <si>
     <t>Buff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log: "鱼人领军init"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"if:1,1"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2146,13 +2150,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2171,52 +2176,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B1" t="s">
         <v>573</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>574</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>575</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>576</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>577</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>578</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>579</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>582</v>
+      </c>
+      <c r="J1" t="s">
+        <v>583</v>
+      </c>
+      <c r="K1" t="s">
+        <v>584</v>
+      </c>
+      <c r="L1" t="s">
+        <v>585</v>
+      </c>
+      <c r="M1" t="s">
+        <v>586</v>
+      </c>
+      <c r="N1" t="s">
+        <v>587</v>
+      </c>
+      <c r="O1" t="s">
         <v>580</v>
       </c>
-      <c r="I1" t="s">
-        <v>583</v>
-      </c>
-      <c r="J1" t="s">
-        <v>584</v>
-      </c>
-      <c r="K1" t="s">
-        <v>585</v>
-      </c>
-      <c r="L1" t="s">
-        <v>586</v>
-      </c>
-      <c r="M1" t="s">
-        <v>587</v>
-      </c>
-      <c r="N1" t="s">
-        <v>588</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>581</v>
-      </c>
-      <c r="P1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>6</v>
@@ -2282,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2315,6 +2320,9 @@
       </c>
       <c r="K5" s="1">
         <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>589</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Revert "Revert "Revert "feat: the first card using OJ worked!"""
This reverts commit 3f5e8c588896fa39535b38daaf2293a7f9c78e3a.
</commit_message>
<xml_diff>
--- a/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
+++ b/iyingdiBattleGround/Assets/StreamingAssets/Mods/Buildin/Card/card.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\iyingdiBattleGround\iyingdiBattleGround\Assets\StreamingAssets\Mods\Buildin\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1156A42-582F-47A7-B8C9-5760A1AFD45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5165B-5DF7-4D76-94F8-C34E99771F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="590">
   <si>
     <t>鱼人招潮者</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1749,6 +1749,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>WhenMinionSummon: if:target.isType:"鱼人": host.AddBuff:“加一攻”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>//唯一名称0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1814,14 +1818,6 @@
   </si>
   <si>
     <t>Buff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Log: "鱼人领军init"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"if:1,1"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2150,14 +2146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2176,52 +2171,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="I1" t="s">
+        <v>583</v>
+      </c>
+      <c r="J1" t="s">
+        <v>584</v>
+      </c>
+      <c r="K1" t="s">
+        <v>585</v>
+      </c>
+      <c r="L1" t="s">
+        <v>586</v>
+      </c>
+      <c r="M1" t="s">
+        <v>587</v>
+      </c>
+      <c r="N1" t="s">
+        <v>588</v>
+      </c>
+      <c r="O1" t="s">
+        <v>581</v>
+      </c>
+      <c r="P1" t="s">
         <v>582</v>
-      </c>
-      <c r="J1" t="s">
-        <v>583</v>
-      </c>
-      <c r="K1" t="s">
-        <v>584</v>
-      </c>
-      <c r="L1" t="s">
-        <v>585</v>
-      </c>
-      <c r="M1" t="s">
-        <v>586</v>
-      </c>
-      <c r="N1" t="s">
-        <v>587</v>
-      </c>
-      <c r="O1" t="s">
-        <v>580</v>
-      </c>
-      <c r="P1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2271,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>6</v>
@@ -2287,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2320,9 +2315,6 @@
       </c>
       <c r="K5" s="1">
         <v>3</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>589</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>

</xml_diff>